<commit_message>
validacao final german credit
</commit_message>
<xml_diff>
--- a/reports/metricas.xlsx
+++ b/reports/metricas.xlsx
@@ -1,21 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10713"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11108"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/fabricio/Dropbox/workspaces/ml-espm/reports/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{37295AE5-B76F-124E-AE6A-6DBB61CD5264}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6261B032-CD18-E54E-86AE-ADF215117CB7}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="20" yWindow="480" windowWidth="29980" windowHeight="14900" xr2:uid="{3E4E30F9-D890-944D-9F13-564EC4020977}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="181029"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -26,6 +26,7 @@
         <xcalcf:feature name="microsoft.com:Single"/>
         <xcalcf:feature name="microsoft.com:FV"/>
         <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
       </xcalcf:calcFeatures>
     </ext>
   </extLst>
@@ -170,13 +171,13 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Good" xfId="1" builtinId="26"/>
@@ -495,7 +496,7 @@
   <dimension ref="A4:P29"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="C2" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <selection activeCell="J9" sqref="J9"/>
+      <selection activeCell="E16" sqref="E16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -562,10 +563,10 @@
       </c>
     </row>
     <row r="7" spans="1:16" x14ac:dyDescent="0.2">
-      <c r="J7" s="2" t="s">
+      <c r="J7" s="4" t="s">
         <v>14</v>
       </c>
-      <c r="K7" s="2"/>
+      <c r="K7" s="4"/>
     </row>
     <row r="8" spans="1:16" x14ac:dyDescent="0.2">
       <c r="J8" s="1" t="s">
@@ -585,7 +586,7 @@
       <c r="I9" t="s">
         <v>11</v>
       </c>
-      <c r="J9" s="4">
+      <c r="J9" s="2">
         <v>172</v>
       </c>
       <c r="K9">
@@ -615,7 +616,7 @@
       <c r="J10">
         <v>258</v>
       </c>
-      <c r="K10" s="4">
+      <c r="K10" s="2">
         <v>370</v>
       </c>
       <c r="L10">
@@ -667,10 +668,10 @@
       </c>
     </row>
     <row r="16" spans="1:16" x14ac:dyDescent="0.2">
-      <c r="J16" s="2" t="s">
+      <c r="J16" s="4" t="s">
         <v>14</v>
       </c>
-      <c r="K16" s="2"/>
+      <c r="K16" s="4"/>
     </row>
     <row r="17" spans="8:16" x14ac:dyDescent="0.2">
       <c r="J17" s="1" t="s">
@@ -687,7 +688,7 @@
       <c r="I18" t="s">
         <v>11</v>
       </c>
-      <c r="J18" s="4" t="s">
+      <c r="J18" s="2" t="s">
         <v>15</v>
       </c>
       <c r="K18" t="s">
@@ -702,15 +703,15 @@
       <c r="J19" t="s">
         <v>18</v>
       </c>
-      <c r="K19" s="4" t="s">
+      <c r="K19" s="2" t="s">
         <v>16</v>
       </c>
     </row>
     <row r="23" spans="8:16" x14ac:dyDescent="0.2">
-      <c r="J23" s="2" t="s">
+      <c r="J23" s="4" t="s">
         <v>14</v>
       </c>
-      <c r="K23" s="2"/>
+      <c r="K23" s="4"/>
     </row>
     <row r="24" spans="8:16" x14ac:dyDescent="0.2">
       <c r="J24" s="1" t="s">
@@ -727,7 +728,7 @@
       <c r="I25" t="s">
         <v>11</v>
       </c>
-      <c r="J25" s="4">
+      <c r="J25" s="2">
         <v>270</v>
       </c>
       <c r="K25">
@@ -757,7 +758,7 @@
       <c r="J26">
         <v>8</v>
       </c>
-      <c r="K26" s="4">
+      <c r="K26" s="2">
         <v>620</v>
       </c>
       <c r="L26">
@@ -807,12 +808,12 @@
     </row>
   </sheetData>
   <mergeCells count="6">
+    <mergeCell ref="H25:H26"/>
     <mergeCell ref="H9:H10"/>
     <mergeCell ref="J7:K7"/>
     <mergeCell ref="J16:K16"/>
     <mergeCell ref="H18:H19"/>
     <mergeCell ref="J23:K23"/>
-    <mergeCell ref="H25:H26"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>